<commit_message>
archivos para Excel, Formato condicional
</commit_message>
<xml_diff>
--- a/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/18 - FORMATO CONDICIONAL/FCondicional 04.xlsx
+++ b/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/18 - FORMATO CONDICIONAL/FCondicional 04.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18915" windowHeight="11820"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="18915" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -113,11 +113,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;Tm&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +254,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -332,6 +337,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -366,6 +372,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -541,414 +548,414 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H4" sqref="H4:H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="3" spans="1:8" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B4" s="5">
         <v>100</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C4" s="5">
         <v>128</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D4" s="5">
         <v>137</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E4" s="5">
         <v>179</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F4" s="5">
         <v>127</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G4" s="5">
         <v>160</v>
       </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B5" s="5">
         <v>108</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C5" s="5">
         <v>141</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D5" s="5">
         <v>118</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E5" s="5">
         <v>192</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F5" s="5">
         <v>152</v>
-      </c>
-      <c r="G3" s="5">
-        <v>200</v>
-      </c>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5">
-        <v>141</v>
-      </c>
-      <c r="C4" s="5">
-        <v>169</v>
-      </c>
-      <c r="D4" s="5">
-        <v>153</v>
-      </c>
-      <c r="E4" s="5">
-        <v>116</v>
-      </c>
-      <c r="F4" s="5">
-        <v>119</v>
-      </c>
-      <c r="G4" s="5">
-        <v>175</v>
-      </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5">
-        <v>105</v>
-      </c>
-      <c r="C5" s="5">
-        <v>198</v>
-      </c>
-      <c r="D5" s="5">
-        <v>133</v>
-      </c>
-      <c r="E5" s="5">
-        <v>106</v>
-      </c>
-      <c r="F5" s="5">
-        <v>158</v>
       </c>
       <c r="G5" s="5">
         <v>200</v>
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>141</v>
+      </c>
+      <c r="C6" s="5">
+        <v>169</v>
+      </c>
+      <c r="D6" s="5">
+        <v>153</v>
+      </c>
+      <c r="E6" s="5">
+        <v>116</v>
+      </c>
+      <c r="F6" s="5">
+        <v>119</v>
+      </c>
+      <c r="G6" s="5">
+        <v>175</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5">
+        <v>105</v>
+      </c>
+      <c r="C7" s="5">
+        <v>198</v>
+      </c>
+      <c r="D7" s="5">
+        <v>133</v>
+      </c>
+      <c r="E7" s="5">
+        <v>106</v>
+      </c>
+      <c r="F7" s="5">
+        <v>158</v>
+      </c>
+      <c r="G7" s="5">
+        <v>200</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B8" s="5">
         <v>188</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C8" s="5">
         <v>175</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D8" s="5">
         <v>190</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E8" s="5">
         <v>114</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F8" s="5">
         <v>138</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G8" s="5">
         <v>150</v>
       </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="4" t="s">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B9" s="5">
         <v>128</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C9" s="5">
         <v>155</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D9" s="5">
         <v>119</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E9" s="5">
         <v>174</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F9" s="5">
         <v>182</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G9" s="5">
         <v>188</v>
       </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="4" t="s">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B10" s="5">
         <v>160</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C10" s="5">
         <v>134</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D10" s="5">
         <v>124</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E10" s="5">
         <v>119</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F10" s="5">
         <v>179</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G10" s="5">
         <v>149</v>
       </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="4" t="s">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B11" s="5">
         <v>184</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C11" s="5">
         <v>114</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D11" s="5">
         <v>181</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E11" s="5">
         <v>179</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F11" s="5">
         <v>142</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G11" s="5">
         <v>179</v>
       </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="4" t="s">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B12" s="5">
         <v>108</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C12" s="5">
         <v>138</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D12" s="5">
         <v>114</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E12" s="5">
         <v>181</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F12" s="5">
         <v>199</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G12" s="5">
         <v>178</v>
       </c>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="4" t="s">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B13" s="5">
         <v>183</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C13" s="5">
         <v>169</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D13" s="5">
         <v>124</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E13" s="5">
         <v>192</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F13" s="5">
         <v>146</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G13" s="5">
         <v>108</v>
       </c>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="4" t="s">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B14" s="5">
         <v>199</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C14" s="5">
         <v>192</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D14" s="5">
         <v>169</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E14" s="5">
         <v>183</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F14" s="5">
         <v>167</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G14" s="5">
         <v>199</v>
       </c>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="4" t="s">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B15" s="5">
         <v>178</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C15" s="5">
         <v>165</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D15" s="5">
         <v>139</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E15" s="5">
         <v>167</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F15" s="5">
         <v>185</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G15" s="5">
         <v>129</v>
       </c>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="4" t="s">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B16" s="5">
         <v>143</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C16" s="5">
         <v>198</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D16" s="5">
         <v>128</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E16" s="5">
         <v>105</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F16" s="5">
         <v>129</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G16" s="5">
         <v>161</v>
       </c>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="4" t="s">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B17" s="5">
         <v>197</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C17" s="5">
         <v>123</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D17" s="5">
         <v>149</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E17" s="5">
         <v>195</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F17" s="5">
         <v>127</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G17" s="5">
         <v>197</v>
       </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="4" t="s">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B18" s="5">
         <v>184</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C18" s="5">
         <v>140</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D18" s="5">
         <v>186</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E18" s="5">
         <v>117</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F18" s="5">
         <v>122</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G18" s="5">
         <v>101</v>
       </c>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="7" t="s">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>